<commit_message>
Update collected throughput data with >100MB file
</commit_message>
<xml_diff>
--- a/ProgrammingAssignment2/throughput_data.xlsx
+++ b/ProgrammingAssignment2/throughput_data.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding\ProgrammingAssignment2\ProgrammingAssignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA1FA560-F927-46C5-9BA8-CBCDA5C8967F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B60668-F5FC-4BE5-8334-8A140429632A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{88FC57AD-6680-4480-BD0F-D23D18D13B8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CP1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -29,12 +26,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">file name </t>
   </si>
@@ -42,13 +42,31 @@
     <t>file size (KB)</t>
   </si>
   <si>
+    <t>CP1 time taken (ms)</t>
+  </si>
+  <si>
+    <t>CP1 time taken (s)</t>
+  </si>
+  <si>
+    <t>CP1 throughput (KB/s)</t>
+  </si>
+  <si>
+    <t>CP2 time taken(ms)</t>
+  </si>
+  <si>
+    <t>CP2 time taken (s)</t>
+  </si>
+  <si>
+    <t>CP2 throughput (KB/s)</t>
+  </si>
+  <si>
+    <t>tiny.bin</t>
+  </si>
+  <si>
     <t>100.txt</t>
   </si>
   <si>
-    <t>CP1 time taken (ms)</t>
-  </si>
-  <si>
-    <t>CP2 time taken(ms)</t>
+    <t>200.txt</t>
   </si>
   <si>
     <t>500.txt</t>
@@ -69,55 +87,74 @@
     <t>100000.txt</t>
   </si>
   <si>
-    <t>200.txt</t>
-  </si>
-  <si>
-    <t>02 平行世界.mp3</t>
-  </si>
-  <si>
-    <t>CP1 time taken (s)</t>
-  </si>
-  <si>
-    <t>tiny.bin</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">02 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Source Han Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t>平行世界</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>.mp3</t>
+    </r>
+  </si>
+  <si>
+    <t>tsetup.2.4.3.exe</t>
+  </si>
+  <si>
+    <t>michael-hampton-figure-drawing-design-and-invention-1.pdf</t>
   </si>
   <si>
     <t>19 JALAN DAPAT, JOHOR BAHRU 600-C.tif</t>
   </si>
   <si>
-    <t>tsetup.2.4.3.exe</t>
-  </si>
-  <si>
-    <t>CP2 time taken (s)</t>
-  </si>
-  <si>
-    <t>michael-hampton-figure-drawing-design-and-invention-1.pdf</t>
-  </si>
-  <si>
-    <t>CP1 throughput (KB/s)</t>
-  </si>
-  <si>
-    <t>CP2 throughput (KB/s)</t>
+    <t>MVI_9870.mp4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Source Han Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,15 +177,84 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFD9D9D9"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFC000"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF595959"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF264478"/>
+      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -165,43 +271,31 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-MY"/>
-              <a:t>Throughput Comparison between</a:t>
+              <a:rPr lang="en-MY" sz="1400" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Throughput Comparison between CP1 and CP2</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-MY" baseline="0"/>
-              <a:t> CP1 and CP2</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-MY"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -211,28 +305,7 @@
         <a:ln>
           <a:noFill/>
         </a:ln>
-        <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -241,7 +314,7 @@
         <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -255,23 +328,60 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="28440">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:srgbClr val="FFC000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'CP1'!$B$2:$B$14</c:f>
+              <c:f>'CP1'!$B$2:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2.9000000000000001E-2</c:v>
                 </c:pt>
@@ -310,16 +420,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>56617</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>133712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'CP1'!$E$2:$E$14</c:f>
+              <c:f>'CP1'!$E$2:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>10.025582520915441</c:v>
                 </c:pt>
@@ -358,6 +471,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>151.85139530698459</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>154.25106861606147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -365,12 +481,12 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-2F3A-447C-BE3A-4792F80A4E95}"/>
+              <c16:uniqueId val="{00000000-3DFE-41F4-AB3F-C748EFC218F1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="6"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
@@ -384,25 +500,60 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="28440">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
+                <a:srgbClr val="264478"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'CP1'!$B$2:$B$14</c:f>
+              <c:f>'CP1'!$B$2:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2.9000000000000001E-2</c:v>
                 </c:pt>
@@ -441,16 +592,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>56617</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>133712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'CP1'!$H$2:$H$14</c:f>
+              <c:f>'CP1'!$H$2:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>11.393548894039997</c:v>
                 </c:pt>
@@ -489,6 +643,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1102.8346836745434</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>992.32222589476282</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -496,7 +653,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-2F3A-447C-BE3A-4792F80A4E95}"/>
+              <c16:uniqueId val="{00000001-3DFE-41F4-AB3F-C748EFC218F1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -508,12 +665,19 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="585629304"/>
-        <c:axId val="585628664"/>
+        <c:axId val="39872966"/>
+        <c:axId val="31120222"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="585629304"/>
+        <c:axId val="39872966"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -522,31 +686,26 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:srgbClr val="595959"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-MY"/>
-                  <a:t>File Size</a:t>
+                  <a:rPr lang="en-MY" sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>File Size (KB)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-MY" baseline="0"/>
-                  <a:t> (KB)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-MY"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -556,75 +715,44 @@
             <a:ln>
               <a:noFill/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:ln w="9360">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
-          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="585628664"/>
+        <c:crossAx val="31120222"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="585628664"/>
+        <c:axId val="31120222"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,59 +760,47 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:ln w="9360">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:noFill/>
-          <a:ln>
+          <a:ln w="6480">
             <a:noFill/>
           </a:ln>
-          <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="595959"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="585629304"/>
+        <c:crossAx val="39872966"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
-        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
@@ -695,23 +811,17 @@
         <a:ln>
           <a:noFill/>
         </a:ln>
-        <a:effectLst/>
       </c:spPr>
       <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:bodyPr/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:srgbClr val="595959"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -720,40 +830,19 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <a:ln w="9360">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:srgbClr val="D9D9D9"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
-    <a:effectLst/>
   </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -762,583 +851,27 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3048000</xdr:colOff>
+      <xdr:colOff>3048120</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>61911</xdr:rowOff>
+      <xdr:rowOff>62280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>142874</xdr:rowOff>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{033496E8-F4DA-4858-92F7-7331CABC27AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1655,11 +1188,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5368FCF5-31CF-4B0E-83A6-80F53D8224CA}">
-  <dimension ref="A1:H14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,6 +1204,7 @@
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="18.140625" customWidth="1"/>
     <col min="8" max="8" width="24.28515625" customWidth="1"/>
+    <col min="9" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1681,27 +1215,27 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>2.9000000000000001E-2</v>
@@ -1710,28 +1244,28 @@
         <v>2.8925999999999998</v>
       </c>
       <c r="D2">
-        <f xml:space="preserve"> C2/1000</f>
+        <f t="shared" ref="D2:D15" si="0">C2/1000</f>
         <v>2.8925999999999999E-3</v>
       </c>
       <c r="E2">
-        <f>B2/D2</f>
+        <f t="shared" ref="E2:E15" si="1">B2/D2</f>
         <v>10.025582520915441</v>
       </c>
       <c r="F2">
         <v>2.5453000000000001</v>
       </c>
       <c r="G2">
-        <f xml:space="preserve"> F2/1000</f>
+        <f t="shared" ref="G2:G15" si="2">F2/1000</f>
         <v>2.5452999999999999E-3</v>
       </c>
       <c r="H2">
-        <f>B2/G2</f>
+        <f t="shared" ref="H2:H15" si="3">B2/G2</f>
         <v>11.393548894039997</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -1740,28 +1274,28 @@
         <v>74.123699999999999</v>
       </c>
       <c r="D3">
-        <f xml:space="preserve"> C3/1000</f>
+        <f t="shared" si="0"/>
         <v>7.4123700000000001E-2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E14" si="0">B3/D3</f>
+        <f t="shared" si="1"/>
         <v>67.454808650944301</v>
       </c>
       <c r="F3">
         <v>10.3543</v>
       </c>
       <c r="G3">
-        <f xml:space="preserve"> F3/1000</f>
+        <f t="shared" si="2"/>
         <v>1.03543E-2</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H14" si="1">B3/G3</f>
+        <f t="shared" si="3"/>
         <v>482.89116598900938</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>9</v>
@@ -1770,11 +1304,11 @@
         <v>78.609800000000007</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:G14" si="2" xml:space="preserve"> C4/1000</f>
+        <f t="shared" si="0"/>
         <v>7.8609800000000007E-2</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>114.48954201638981</v>
       </c>
       <c r="F4">
@@ -1785,13 +1319,13 @@
         <v>1.4570100000000001E-2</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>617.70337883748221</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>23</v>
@@ -1800,11 +1334,11 @@
         <v>150.05009999999999</v>
       </c>
       <c r="D5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.15005009999999999</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>153.2821370995421</v>
       </c>
       <c r="F5">
@@ -1815,13 +1349,13 @@
         <v>3.9074800000000007E-2</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>588.61465701679845</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>45</v>
@@ -1830,11 +1364,11 @@
         <v>290.82679999999999</v>
       </c>
       <c r="D6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.2908268</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>154.73126960789034</v>
       </c>
       <c r="F6">
@@ -1845,13 +1379,13 @@
         <v>5.4153699999999999E-2</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>830.96815176063683</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>225</v>
@@ -1860,11 +1394,11 @@
         <v>1298.905</v>
       </c>
       <c r="D7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1.298905</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>173.22282999911465</v>
       </c>
       <c r="F7">
@@ -1875,13 +1409,13 @@
         <v>0.2042438</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1101.6246270388624</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>450</v>
@@ -1890,11 +1424,11 @@
         <v>2320.7428</v>
       </c>
       <c r="D8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>2.3207428000000001</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>193.90343471064523</v>
       </c>
       <c r="F8">
@@ -1905,13 +1439,13 @@
         <v>0.30750459999999996</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1463.3927427427104</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>2247</v>
@@ -1920,11 +1454,11 @@
         <v>13270.960300000001</v>
       </c>
       <c r="D9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>13.2709603</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>169.3170614036122</v>
       </c>
       <c r="F9">
@@ -1935,13 +1469,13 @@
         <v>1.5495490999999999</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1450.0992579067033</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>4493</v>
@@ -1950,11 +1484,11 @@
         <v>24564.982800000002</v>
       </c>
       <c r="D10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>24.564982800000003</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>182.902631627326</v>
       </c>
       <c r="F10">
@@ -1965,13 +1499,13 @@
         <v>3.8243733000000004</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1174.8330112021229</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>11017</v>
@@ -1980,11 +1514,11 @@
         <v>59866.025999999998</v>
       </c>
       <c r="D11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>59.866025999999998</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>184.0275818541889</v>
       </c>
       <c r="F11">
@@ -1995,13 +1529,13 @@
         <v>11.2861805</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>976.14954855630742</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>24887</v>
@@ -2010,11 +1544,11 @@
         <v>174198.37580000001</v>
       </c>
       <c r="D12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>174.19837580000001</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>142.86585558394168</v>
       </c>
       <c r="F12">
@@ -2025,13 +1559,13 @@
         <v>22.607517199999997</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1100.8285332632636</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>46471</v>
@@ -2040,11 +1574,11 @@
         <v>303022.6263</v>
       </c>
       <c r="D13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>303.02262630000001</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>153.35818505510721</v>
       </c>
       <c r="F13">
@@ -2055,13 +1589,13 @@
         <v>41.334410099999999</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1124.2690989800772</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>56617</v>
@@ -2070,11 +1604,11 @@
         <v>372844.7795</v>
       </c>
       <c r="D14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>372.84477950000002</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>151.85139530698459</v>
       </c>
       <c r="F14">
@@ -2085,13 +1619,43 @@
         <v>51.337703500000003</v>
       </c>
       <c r="H14">
+        <f t="shared" si="3"/>
+        <v>1102.8346836745434</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>133712</v>
+      </c>
+      <c r="C15">
+        <v>866846.50679999997</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>866.84650679999993</v>
+      </c>
+      <c r="E15" s="2">
         <f t="shared" si="1"/>
-        <v>1102.8346836745434</v>
+        <v>154.25106861606147</v>
+      </c>
+      <c r="F15">
+        <v>134746.55360000001</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="2"/>
+        <v>134.74655360000003</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="3"/>
+        <v>992.32222589476282</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>